<commit_message>
Cajamar experiments with large parameter variance
</commit_message>
<xml_diff>
--- a/extensions/icdm2016/doc-Experiments/RecapExperiments.xlsx
+++ b/extensions/icdm2016/doc-Experiments/RecapExperiments.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22240" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="27320" windowHeight="14000" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CajaMar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>2016-bs100</t>
   </si>
@@ -295,6 +295,9 @@
   </si>
   <si>
     <t>2016-bs5k</t>
+  </si>
+  <si>
+    <t>2016 -bs50K-var100</t>
   </si>
 </sst>
 </file>
@@ -343,8 +346,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -383,7 +392,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -401,6 +410,9 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -418,6 +430,9 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,7 +465,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$1</c:f>
+              <c:f>CajaMar!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -464,7 +479,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$2:$J$85</c:f>
+              <c:f>CajaMar!$J$2:$J$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -730,7 +745,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$1</c:f>
+              <c:f>CajaMar!$K$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -744,7 +759,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$2:$K$85</c:f>
+              <c:f>CajaMar!$K$2:$K$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -999,6 +1014,286 @@
                 </c:pt>
                 <c:pt idx="83">
                   <c:v>-10.5491300812397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>CajaMar!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2016 -bs50K-var100</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>CajaMar!$L$2:$L$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="84"/>
+                <c:pt idx="0">
+                  <c:v>-10.5295297990214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10.5295297452378</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10.5265684034782</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-10.5291608719122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-10.5272475085439</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-10.5249850565216</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-10.5277631905843</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-10.5300247711471</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-10.5283503265045</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-10.5289016704537</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-10.5297574026765</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-10.5284454991767</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-10.5295929873975</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-10.52914985808</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-10.5255152172029</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-10.5294779354348</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-10.5292535170353</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-10.5296518819665</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-10.5278162551683</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-10.5286805746159</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-10.5296704207434</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-10.5296542009474</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-10.5293287050621</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-10.5272470345327</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-10.5296960848091</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-10.5296691708443</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-10.5243099064213</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-10.5203635022738</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-10.5285900311772</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-10.5296321817144</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-10.5271564848567</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-10.5295447782768</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-10.529555128269</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-10.529539655469</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-10.529535217774</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-10.5290329539835</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-10.5295887231577</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-10.5285723104551</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-10.5295211059314</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-10.5294999817251</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-10.529516106207</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-10.5295828621045</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-10.5277700038646</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-10.5296941999365</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-10.5296497045668</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-10.5296066512804</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-10.5283836219489</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-10.5296719639713</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-10.5296341957985</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-10.5286142109481</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-10.529653313002</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>-10.5294707097859</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>-10.5289360919585</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>-10.5294514586903</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>-10.5296099977802</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>-10.5296028932878</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>-10.5294236271733</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>-10.5291109704603</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-10.5270229041668</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-10.5287315013182</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>-10.5289628243953</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>-10.5286651127254</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>-10.5297269346253</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>-10.5294528817493</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>-10.5294376832723</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>-10.5265130980491</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>-10.5294955655476</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>-10.5287402997003</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>-10.5289479936413</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>-10.5297588710333</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-10.5293479417494</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>-10.5295068972336</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-10.52594816526</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>-10.5297469835051</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>-10.5297691290718</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>-10.5293876430523</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>-10.5295024722024</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>-10.5295985766354</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>-10.5297418059198</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>-10.528698078919</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>-10.5273978866071</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-10.5297668824527</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>-10.5294256348174</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>-10.5290665593931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1015,8 +1310,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2118618408"/>
-        <c:axId val="-2115075336"/>
+        <c:axId val="2124051256"/>
+        <c:axId val="2123789048"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1026,7 +1321,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$1</c:f>
+              <c:f>CajaMar!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1035,12 +1330,22 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$2:$I$85</c:f>
+              <c:f>CajaMar!$I$2:$I$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -1311,11 +1616,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2103867256"/>
-        <c:axId val="-2103869048"/>
+        <c:axId val="2111528120"/>
+        <c:axId val="2073321944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2118618408"/>
+        <c:axId val="2124051256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1324,7 +1629,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2115075336"/>
+        <c:crossAx val="2123789048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1332,7 +1637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2115075336"/>
+        <c:axId val="2123789048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,14 +1648,15 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118618408"/>
+        <c:crossAx val="2124051256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2103869048"/>
+        <c:axId val="2073321944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="8.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="r"/>
@@ -1358,12 +1664,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103867256"/>
+        <c:crossAx val="2111528120"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2103867256"/>
+        <c:axId val="2111528120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1678,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2103869048"/>
+        <c:crossAx val="2073321944"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1425,7 +1732,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$1</c:f>
+              <c:f>CajaMar!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1439,7 +1746,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$85</c:f>
+              <c:f>CajaMar!$F$2:$F$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -1710,11 +2017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2121625960"/>
-        <c:axId val="2081764584"/>
+        <c:axId val="2126034488"/>
+        <c:axId val="2126037496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2121625960"/>
+        <c:axId val="2126034488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,7 +2030,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2081764584"/>
+        <c:crossAx val="2126037496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1731,7 +2038,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081764584"/>
+        <c:axId val="2126037496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,7 +2049,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2121625960"/>
+        <c:crossAx val="2126034488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1789,7 +2096,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>CajaMar!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1803,7 +2110,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$85</c:f>
+              <c:f>CajaMar!$B$2:$B$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -2069,7 +2376,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>CajaMar!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2083,7 +2390,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$85</c:f>
+              <c:f>CajaMar!$C$2:$C$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -2354,8 +2661,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2101409080"/>
-        <c:axId val="-2101399160"/>
+        <c:axId val="2126273512"/>
+        <c:axId val="2126268696"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2365,7 +2672,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>CajaMar!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2379,7 +2686,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$85</c:f>
+              <c:f>CajaMar!$D$2:$D$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -2585,7 +2892,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$1</c:f>
+              <c:f>CajaMar!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2599,7 +2906,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$85</c:f>
+              <c:f>CajaMar!$E$2:$E$85</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="84"/>
@@ -2870,11 +3177,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2122725912"/>
-        <c:axId val="2121411304"/>
+        <c:axId val="2126339832"/>
+        <c:axId val="2126297448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2101409080"/>
+        <c:axId val="2126273512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2883,7 +3190,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2101399160"/>
+        <c:crossAx val="2126268696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2891,7 +3198,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101399160"/>
+        <c:axId val="2126268696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2902,12 +3209,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2101409080"/>
+        <c:crossAx val="2126273512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2121411304"/>
+        <c:axId val="2126297448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2917,12 +3224,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122725912"/>
+        <c:crossAx val="2126339832"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2122725912"/>
+        <c:axId val="2126339832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2931,7 +3238,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121411304"/>
+        <c:crossAx val="2126297448"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3372,10 +3680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q49" sqref="Q49"/>
+    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3383,9 +3691,10 @@
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="B1" t="s">
         <v>88</v>
       </c>
@@ -3410,8 +3719,11 @@
       <c r="K1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3442,8 +3754,11 @@
       <c r="K2">
         <v>-10.5489920573081</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2">
+        <v>-10.5295297990214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3474,8 +3789,11 @@
       <c r="K3">
         <v>-10.548992006452201</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3">
+        <v>-10.5295297452378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3506,8 +3824,11 @@
       <c r="K4">
         <v>-10.5455018065165</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4">
+        <v>-10.526568403478199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3538,8 +3859,11 @@
       <c r="K5">
         <v>-10.549359467146701</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5">
+        <v>-10.5291608719122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3570,8 +3894,11 @@
       <c r="K6">
         <v>-10.5469159807661</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6">
+        <v>-10.527247508543899</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3602,8 +3929,11 @@
       <c r="K7">
         <v>-10.5451240603277</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7">
+        <v>-10.524985056521601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3634,8 +3964,11 @@
       <c r="K8">
         <v>-10.547904872731699</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8">
+        <v>-10.527763190584301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3666,8 +3999,11 @@
       <c r="K9">
         <v>-10.5503750698941</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9">
+        <v>-10.530024771147099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3698,8 +4034,11 @@
       <c r="K10">
         <v>-10.548677018392899</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="L10">
+        <v>-10.5283503265045</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3730,8 +4069,11 @@
       <c r="K11">
         <v>-10.5491711967366</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L11">
+        <v>-10.528901670453701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3762,8 +4104,11 @@
       <c r="K12">
         <v>-10.5497866571895</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12">
+        <v>-10.5297574026765</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3794,8 +4139,11 @@
       <c r="K13">
         <v>-10.548754145957901</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13">
+        <v>-10.5284454991767</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3826,8 +4174,11 @@
       <c r="K14">
         <v>-10.5496915352531</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="L14">
+        <v>-10.5295929873975</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3858,8 +4209,11 @@
       <c r="K15">
         <v>-10.5493179963711</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15">
+        <v>-10.52914985808</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3890,8 +4244,11 @@
       <c r="K16">
         <v>-10.545120984655799</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16">
+        <v>-10.5255152172029</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3922,8 +4279,11 @@
       <c r="K17">
         <v>-10.5498915724264</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17">
+        <v>-10.5294779354348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3954,8 +4314,11 @@
       <c r="K18">
         <v>-10.5493198926426</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="L18">
+        <v>-10.529253517035301</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3986,8 +4349,11 @@
       <c r="K19">
         <v>-10.5498391922343</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19">
+        <v>-10.529651881966499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4018,8 +4384,11 @@
       <c r="K20">
         <v>-10.5479503377502</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="L20">
+        <v>-10.5278162551683</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4050,8 +4419,11 @@
       <c r="K21">
         <v>-10.5488472611425</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="L21">
+        <v>-10.528680574615899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4082,8 +4454,11 @@
       <c r="K22">
         <v>-10.5498650139755</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22">
+        <v>-10.5296704207434</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4114,8 +4489,11 @@
       <c r="K23">
         <v>-10.549761171918</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23">
+        <v>-10.5296542009474</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4146,8 +4524,11 @@
       <c r="K24">
         <v>-10.549416427033499</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="L24">
+        <v>-10.529328705062101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4178,8 +4559,11 @@
       <c r="K25">
         <v>-10.5469152729888</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="L25">
+        <v>-10.527247034532699</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4210,8 +4594,11 @@
       <c r="K26">
         <v>-10.550007560804101</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="L26">
+        <v>-10.5296960848091</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4242,8 +4629,11 @@
       <c r="K27">
         <v>-10.549978609437201</v>
       </c>
-    </row>
-    <row r="28" spans="1:11">
+      <c r="L27">
+        <v>-10.529669170844301</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4274,8 +4664,11 @@
       <c r="K28">
         <v>-10.5428726255425</v>
       </c>
-    </row>
-    <row r="29" spans="1:11">
+      <c r="L28">
+        <v>-10.524309906421299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4306,8 +4699,11 @@
       <c r="K29">
         <v>-10.541064453519899</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="L29">
+        <v>-10.520363502273799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4338,8 +4734,11 @@
       <c r="K30">
         <v>-10.5489415062987</v>
       </c>
-    </row>
-    <row r="31" spans="1:11">
+      <c r="L30">
+        <v>-10.528590031177201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4370,8 +4769,11 @@
       <c r="K31">
         <v>-10.550167667582601</v>
       </c>
-    </row>
-    <row r="32" spans="1:11">
+      <c r="L31">
+        <v>-10.529632181714399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4402,8 +4804,11 @@
       <c r="K32">
         <v>-10.5470886337376</v>
       </c>
-    </row>
-    <row r="33" spans="1:11">
+      <c r="L32">
+        <v>-10.5271564848567</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4434,8 +4839,11 @@
       <c r="K33">
         <v>-10.5500639380209</v>
       </c>
-    </row>
-    <row r="34" spans="1:11">
+      <c r="L33">
+        <v>-10.529544778276801</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4466,8 +4874,11 @@
       <c r="K34">
         <v>-10.5500083055534</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
+      <c r="L34">
+        <v>-10.529555128268999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4498,8 +4909,11 @@
       <c r="K35">
         <v>-10.550044010014</v>
       </c>
-    </row>
-    <row r="36" spans="1:11">
+      <c r="L35">
+        <v>-10.529539655469</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4530,8 +4944,11 @@
       <c r="K36">
         <v>-10.5500659911488</v>
       </c>
-    </row>
-    <row r="37" spans="1:11">
+      <c r="L36">
+        <v>-10.529535217774001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4562,8 +4979,11 @@
       <c r="K37">
         <v>-10.5496245226804</v>
       </c>
-    </row>
-    <row r="38" spans="1:11">
+      <c r="L37">
+        <v>-10.529032953983499</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4594,8 +5014,11 @@
       <c r="K38">
         <v>-10.5501450312073</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
+      <c r="L38">
+        <v>-10.529588723157699</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4626,8 +5049,11 @@
       <c r="K39">
         <v>-10.548944309769499</v>
       </c>
-    </row>
-    <row r="40" spans="1:11">
+      <c r="L39">
+        <v>-10.5285723104551</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4658,8 +5084,11 @@
       <c r="K40">
         <v>-10.5500323296197</v>
       </c>
-    </row>
-    <row r="41" spans="1:11">
+      <c r="L40">
+        <v>-10.5295211059314</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4690,8 +5119,11 @@
       <c r="K41">
         <v>-10.550116893758601</v>
       </c>
-    </row>
-    <row r="42" spans="1:11">
+      <c r="L41">
+        <v>-10.529499981725101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4722,8 +5154,11 @@
       <c r="K42">
         <v>-10.550035023487199</v>
       </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="L42">
+        <v>-10.529516106207</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
       <c r="A43">
         <v>41</v>
       </c>
@@ -4754,8 +5189,11 @@
       <c r="K43">
         <v>-10.549990125026101</v>
       </c>
-    </row>
-    <row r="44" spans="1:11">
+      <c r="L43">
+        <v>-10.529582862104499</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4786,8 +5224,11 @@
       <c r="K44">
         <v>-10.5479248069081</v>
       </c>
-    </row>
-    <row r="45" spans="1:11">
+      <c r="L44">
+        <v>-10.5277700038646</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
       <c r="A45">
         <v>43</v>
       </c>
@@ -4818,8 +5259,11 @@
       <c r="K45">
         <v>-10.549989087803599</v>
       </c>
-    </row>
-    <row r="46" spans="1:11">
+      <c r="L45">
+        <v>-10.5296941999365</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4850,8 +5294,11 @@
       <c r="K46">
         <v>-10.5499592316371</v>
       </c>
-    </row>
-    <row r="47" spans="1:11">
+      <c r="L46">
+        <v>-10.5296497045668</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
       <c r="A47">
         <v>45</v>
       </c>
@@ -4882,8 +5329,11 @@
       <c r="K47">
         <v>-10.5500323914211</v>
       </c>
-    </row>
-    <row r="48" spans="1:11">
+      <c r="L47">
+        <v>-10.5296066512804</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4914,8 +5364,11 @@
       <c r="K48">
         <v>-10.548747683110699</v>
       </c>
-    </row>
-    <row r="49" spans="1:11">
+      <c r="L48">
+        <v>-10.528383621948899</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
       <c r="A49">
         <v>47</v>
       </c>
@@ -4946,8 +5399,11 @@
       <c r="K49">
         <v>-10.5499778883938</v>
       </c>
-    </row>
-    <row r="50" spans="1:11">
+      <c r="L49">
+        <v>-10.5296719639713</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4978,8 +5434,11 @@
       <c r="K50">
         <v>-10.550069856947101</v>
       </c>
-    </row>
-    <row r="51" spans="1:11">
+      <c r="L50">
+        <v>-10.529634195798501</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>49</v>
       </c>
@@ -5010,8 +5469,11 @@
       <c r="K51">
         <v>-10.5490471493939</v>
       </c>
-    </row>
-    <row r="52" spans="1:11">
+      <c r="L51">
+        <v>-10.528614210948099</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>50</v>
       </c>
@@ -5042,8 +5504,11 @@
       <c r="K52">
         <v>-10.549969809042199</v>
       </c>
-    </row>
-    <row r="53" spans="1:11">
+      <c r="L52">
+        <v>-10.529653313001999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>51</v>
       </c>
@@ -5074,8 +5539,11 @@
       <c r="K53">
         <v>-10.5499264370406</v>
       </c>
-    </row>
-    <row r="54" spans="1:11">
+      <c r="L53">
+        <v>-10.529470709785899</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>52</v>
       </c>
@@ -5106,8 +5574,11 @@
       <c r="K54">
         <v>-10.549160132445399</v>
       </c>
-    </row>
-    <row r="55" spans="1:11">
+      <c r="L54">
+        <v>-10.528936091958499</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>53</v>
       </c>
@@ -5138,8 +5609,11 @@
       <c r="K55">
         <v>-10.5496824107981</v>
       </c>
-    </row>
-    <row r="56" spans="1:11">
+      <c r="L55">
+        <v>-10.5294514586903</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>54</v>
       </c>
@@ -5170,8 +5644,11 @@
       <c r="K56">
         <v>-10.549906651643299</v>
       </c>
-    </row>
-    <row r="57" spans="1:11">
+      <c r="L56">
+        <v>-10.5296099977802</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>55</v>
       </c>
@@ -5202,8 +5679,11 @@
       <c r="K57">
         <v>-10.549874261872001</v>
       </c>
-    </row>
-    <row r="58" spans="1:11">
+      <c r="L57">
+        <v>-10.5296028932878</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>56</v>
       </c>
@@ -5234,8 +5714,11 @@
       <c r="K58">
         <v>-10.549617135659901</v>
       </c>
-    </row>
-    <row r="59" spans="1:11">
+      <c r="L58">
+        <v>-10.529423627173299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>57</v>
       </c>
@@ -5266,8 +5749,11 @@
       <c r="K59">
         <v>-10.5492754592746</v>
       </c>
-    </row>
-    <row r="60" spans="1:11">
+      <c r="L59">
+        <v>-10.5291109704603</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
       <c r="A60">
         <v>58</v>
       </c>
@@ -5298,8 +5784,11 @@
       <c r="K60">
         <v>-10.5473379132058</v>
       </c>
-    </row>
-    <row r="61" spans="1:11">
+      <c r="L60">
+        <v>-10.527022904166801</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>59</v>
       </c>
@@ -5330,8 +5819,11 @@
       <c r="K61">
         <v>-10.548919970724301</v>
       </c>
-    </row>
-    <row r="62" spans="1:11">
+      <c r="L61">
+        <v>-10.5287315013182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5362,8 +5854,11 @@
       <c r="K62">
         <v>-10.5493141914524</v>
       </c>
-    </row>
-    <row r="63" spans="1:11">
+      <c r="L62">
+        <v>-10.5289628243953</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>61</v>
       </c>
@@ -5394,8 +5889,11 @@
       <c r="K63">
         <v>-10.5490593273237</v>
       </c>
-    </row>
-    <row r="64" spans="1:11">
+      <c r="L63">
+        <v>-10.528665112725401</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5426,8 +5924,11 @@
       <c r="K64">
         <v>-10.5499598296927</v>
       </c>
-    </row>
-    <row r="65" spans="1:11">
+      <c r="L64">
+        <v>-10.5297269346253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65">
         <v>63</v>
       </c>
@@ -5458,8 +5959,11 @@
       <c r="K65">
         <v>-10.549790661672301</v>
       </c>
-    </row>
-    <row r="66" spans="1:11">
+      <c r="L65">
+        <v>-10.5294528817493</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5487,8 +5991,11 @@
       <c r="K66">
         <v>-10.5497654775103</v>
       </c>
-    </row>
-    <row r="67" spans="1:11">
+      <c r="L66">
+        <v>-10.529437683272301</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
       <c r="A67">
         <v>65</v>
       </c>
@@ -5516,8 +6023,11 @@
       <c r="K67">
         <v>-10.5458728763774</v>
       </c>
-    </row>
-    <row r="68" spans="1:11">
+      <c r="L67">
+        <v>-10.526513098049101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
       <c r="A68">
         <v>66</v>
       </c>
@@ -5545,8 +6055,11 @@
       <c r="K68">
         <v>-10.549809573965801</v>
       </c>
-    </row>
-    <row r="69" spans="1:11">
+      <c r="L68">
+        <v>-10.529495565547601</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
       <c r="A69">
         <v>67</v>
       </c>
@@ -5574,8 +6087,11 @@
       <c r="K69">
         <v>-10.549052043182099</v>
       </c>
-    </row>
-    <row r="70" spans="1:11">
+      <c r="L69">
+        <v>-10.528740299700299</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5603,8 +6119,11 @@
       <c r="K70">
         <v>-10.5491684671596</v>
       </c>
-    </row>
-    <row r="71" spans="1:11">
+      <c r="L70">
+        <v>-10.5289479936413</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
       <c r="A71">
         <v>69</v>
       </c>
@@ -5632,8 +6151,11 @@
       <c r="K71">
         <v>-10.5500463266512</v>
       </c>
-    </row>
-    <row r="72" spans="1:11">
+      <c r="L71">
+        <v>-10.5297588710333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
       <c r="A72">
         <v>70</v>
       </c>
@@ -5661,8 +6183,11 @@
       <c r="K72">
         <v>-10.549708439626601</v>
       </c>
-    </row>
-    <row r="73" spans="1:11">
+      <c r="L72">
+        <v>-10.5293479417494</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12">
       <c r="A73">
         <v>71</v>
       </c>
@@ -5690,8 +6215,11 @@
       <c r="K73">
         <v>-10.549736404234899</v>
       </c>
-    </row>
-    <row r="74" spans="1:11">
+      <c r="L73">
+        <v>-10.529506897233601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74">
         <v>72</v>
       </c>
@@ -5719,8 +6247,11 @@
       <c r="K74">
         <v>-10.546435478342399</v>
       </c>
-    </row>
-    <row r="75" spans="1:11">
+      <c r="L74">
+        <v>-10.525948165260001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75">
         <v>73</v>
       </c>
@@ -5748,8 +6279,11 @@
       <c r="K75">
         <v>-10.5502019996154</v>
       </c>
-    </row>
-    <row r="76" spans="1:11">
+      <c r="L75">
+        <v>-10.529746983505101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12">
       <c r="A76">
         <v>74</v>
       </c>
@@ -5777,8 +6311,11 @@
       <c r="K76">
         <v>-10.5500367624134</v>
       </c>
-    </row>
-    <row r="77" spans="1:11">
+      <c r="L76">
+        <v>-10.5297691290718</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
       <c r="A77">
         <v>75</v>
       </c>
@@ -5806,8 +6343,11 @@
       <c r="K77">
         <v>-10.5498730994537</v>
       </c>
-    </row>
-    <row r="78" spans="1:11">
+      <c r="L77">
+        <v>-10.529387643052299</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
       <c r="A78">
         <v>76</v>
       </c>
@@ -5835,8 +6375,11 @@
       <c r="K78">
         <v>-10.549860160491599</v>
       </c>
-    </row>
-    <row r="79" spans="1:11">
+      <c r="L78">
+        <v>-10.529502472202401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
       <c r="A79">
         <v>77</v>
       </c>
@@ -5864,8 +6407,11 @@
       <c r="K79">
         <v>-10.5497674193722</v>
       </c>
-    </row>
-    <row r="80" spans="1:11">
+      <c r="L79">
+        <v>-10.529598576635401</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12">
       <c r="A80">
         <v>78</v>
       </c>
@@ -5893,8 +6439,11 @@
       <c r="K80">
         <v>-10.5500902564998</v>
       </c>
-    </row>
-    <row r="81" spans="1:11">
+      <c r="L80">
+        <v>-10.5297418059198</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12">
       <c r="A81">
         <v>79</v>
       </c>
@@ -5922,8 +6471,11 @@
       <c r="K81">
         <v>-10.549027453208099</v>
       </c>
-    </row>
-    <row r="82" spans="1:11">
+      <c r="L81">
+        <v>-10.528698078919</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
       <c r="A82">
         <v>80</v>
       </c>
@@ -5951,8 +6503,11 @@
       <c r="K82">
         <v>-10.5474055372671</v>
       </c>
-    </row>
-    <row r="83" spans="1:11">
+      <c r="L82">
+        <v>-10.527397886607099</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
       <c r="A83">
         <v>81</v>
       </c>
@@ -5980,8 +6535,11 @@
       <c r="K83">
         <v>-10.550129742798401</v>
       </c>
-    </row>
-    <row r="84" spans="1:11">
+      <c r="L83">
+        <v>-10.5297668824527</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6009,8 +6567,11 @@
       <c r="K84">
         <v>-10.549815166701601</v>
       </c>
-    </row>
-    <row r="85" spans="1:11">
+      <c r="L84">
+        <v>-10.5294256348174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
       <c r="A85">
         <v>83</v>
       </c>
@@ -6037,6 +6598,9 @@
       </c>
       <c r="K85">
         <v>-10.549130081239699</v>
+      </c>
+      <c r="L85">
+        <v>-10.529066559393099</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Print means in TestGradientBoostingHypothesis and setOutput for NaiveBayesVirtualConceptDriftDetector
</commit_message>
<xml_diff>
--- a/extensions/icdm2016/doc-Experiments/RecapExperiments.xlsx
+++ b/extensions/icdm2016/doc-Experiments/RecapExperiments.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="0" windowWidth="27320" windowHeight="14000" tabRatio="500"/>
+    <workbookView xWindow="-25600" yWindow="0" windowWidth="27320" windowHeight="14000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CajaMar" sheetId="1" r:id="rId1"/>
+    <sheet name="VAR01" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
   <si>
     <t>2016-bs100</t>
   </si>
@@ -298,6 +299,27 @@
   </si>
   <si>
     <t>2016 -bs50K-var100</t>
+  </si>
+  <si>
+    <t>realMean_c0</t>
+  </si>
+  <si>
+    <t>learntMean_c0</t>
+  </si>
+  <si>
+    <t>realMean_c1</t>
+  </si>
+  <si>
+    <t>learntMean_c1</t>
+  </si>
+  <si>
+    <t>meanH</t>
+  </si>
+  <si>
+    <t>Window size 100</t>
+  </si>
+  <si>
+    <t>Window size 1000</t>
   </si>
 </sst>
 </file>
@@ -346,7 +368,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -388,11 +410,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -413,6 +440,7 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -433,6 +461,7 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3263,6 +3292,1398 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>58371.9364778383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58632.4775525353</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57434.134096443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57897.4712765675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58323.0645707848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58771.8698934133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59044.9984139311</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59363.5326881757</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59052.4075783801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59311.1983625028</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59516.3155590386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59752.1073129386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59953.0550646197</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60088.1459457886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59808.7798144426</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59992.0961363341</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60185.7450038501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60354.1163627501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60504.6182548862</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60647.2460622065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>39479.7279197339</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48822.5301810437</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48248.5955955802</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52352.53659223</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54583.8327576876</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56221.7927385</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56969.0199981099</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57880.0448177789</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56103.9155795609</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57437.9010455101</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58240.3320277045</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59092.3167764613</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59637.5006550118</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59847.2653822576</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>57876.5820386284</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>58983.7551721785</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59925.770196199</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60553.844698029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>61002.0718450927</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>61377.888397683</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2110204472"/>
+        <c:axId val="-2141667336"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2110204472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2141667336"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2141667336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2110204472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>76836.3954505686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76351.3634331694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75564.0955256656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79608.99437851339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83451.4538343819</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87653.4194635585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91595.09792142249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95288.2854436375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97178.729157278</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100442.56620784</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102984.150171645</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105194.777652594</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108736.553572516</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>112174.257425742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113405.216317711</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115859.53726513</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>117797.302857142</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>119690.042619139</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121133.374308543</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>122620.029050367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>195988.036349729</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>195990.989752459</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>195988.092283086</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>195994.283361622</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>195998.641944242</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>196002.554692902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>196004.839076042</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>196007.808968012</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>196003.660646463</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>196008.215960754</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>196011.348649587</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>196014.755075036</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>196017.25432917</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>196018.608427878</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>196012.527045716</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>196017.088221838</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>196021.118323578</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>196024.039448333</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>196026.301519179</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>196028.28752524</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2125645416"/>
+        <c:axId val="2125639656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2125645416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2125639656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2125639656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2125645416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>meanH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$E$3:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>13.9545571443096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.5748332600799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.9114314839983</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.1373430951487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.5925449889447</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.1033180330585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.8159565644017</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.445633673574</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11.9481337588558</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.3835365563732</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10.9943996457867</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.5714585465968</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.2620357981649</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.0940710666718</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10.8374129087554</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.2755937896281</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.77924303328439</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.41901821841351</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.14000995270174</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.895220776561571</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2127051976"/>
+        <c:axId val="2126859640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2127051976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2126859640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2126859640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2127051976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$A$26:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>58371.9364778383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58632.4775525353</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57434.134096443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57897.4712765675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58323.0645707848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58771.8698934133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59044.9984139311</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59363.5326881757</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59052.4075783801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59311.1983625028</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59516.3155590386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59752.1073129386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59953.0550646197</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60088.1459457886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59808.7798144426</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59992.0961363341</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60185.7450038501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60354.1163627501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60504.6182548862</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60647.2460622065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$B$26:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>35472.6338299442</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46891.909015302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46781.641359458</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51679.0816661208</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>54165.678055018</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55913.8035640944</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>56690.1072584419</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>57611.8235335768</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>55884.8927492505</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>57180.9061050337</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>57965.1748061819</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>58804.7200898512</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59246.6796659658</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>59385.2101406394</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>57501.1519017676</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>58563.0930704615</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>59491.4345791437</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60113.761717786</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60570.4921872887</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60942.7309156018</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2141509672"/>
+        <c:axId val="-2141630360"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2141509672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2141630360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2141630360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2141509672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$C$26:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>76836.3954505686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76351.3634331694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75564.0955256656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79608.99437851339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83451.4538343819</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87653.4194635585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91595.09792142249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95288.2854436375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97178.729157278</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100442.56620784</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102984.150171645</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105194.777652594</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108736.553572516</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>112174.257425742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113405.216317711</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115859.53726513</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>117797.302857142</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>119690.042619139</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121133.374308543</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>122620.029050367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$D$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$D$26:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>44968.6975982229</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59664.6144134571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62469.9635180786</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73464.1236149361</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80120.78650117179</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85816.9238296359</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90802.5097001127</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95017.3040142183</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97404.8609030494</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100861.251038173</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>103396.494815968</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105460.137963981</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>109149.992737752</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>112321.013735801</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>114509.091171643</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115873.638481811</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>116714.037089879</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>117656.806067122</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>118317.703158651</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>119009.154407696</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2121343224"/>
+        <c:axId val="2121344632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2121343224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121344632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2121344632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121343224"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01'!$E$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>meanH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01'!$E$26:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>16.2521065819409</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.1446648453178</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.3397373173395</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.2147463340334</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.5422990961546</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.0016781511156</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.7144552581047</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.3614266819324</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.8664160653228</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.346090668887</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.9924747667863</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.6023780636563</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.386470849114</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.2947603294558</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.0152620533765</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.5019311749676</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11.0330375794203</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10.6966136697067</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10.4281292991503</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.1987998575596</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2129465512"/>
+        <c:axId val="2127381672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2129465512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2127381672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2127381672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2129465512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3350,6 +4771,191 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3682,7 +5288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G5" workbookViewId="0">
+    <sheetView topLeftCell="G8" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -6613,4 +8219,762 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>58371.936477838302</v>
+      </c>
+      <c r="B3">
+        <v>39479.727919733901</v>
+      </c>
+      <c r="C3">
+        <v>76836.395450568598</v>
+      </c>
+      <c r="D3">
+        <v>195988.03634972899</v>
+      </c>
+      <c r="E3">
+        <v>13.9545571443096</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>58632.477552535303</v>
+      </c>
+      <c r="B4">
+        <v>48822.530181043701</v>
+      </c>
+      <c r="C4">
+        <v>76351.363433169405</v>
+      </c>
+      <c r="D4">
+        <v>195990.98975245899</v>
+      </c>
+      <c r="E4">
+        <v>13.574833260079901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>57434.134096442998</v>
+      </c>
+      <c r="B5">
+        <v>48248.595595580198</v>
+      </c>
+      <c r="C5">
+        <v>75564.095525665602</v>
+      </c>
+      <c r="D5">
+        <v>195988.09228308601</v>
+      </c>
+      <c r="E5">
+        <v>13.9114314839983</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>57897.471276567499</v>
+      </c>
+      <c r="B6">
+        <v>52352.536592229997</v>
+      </c>
+      <c r="C6">
+        <v>79608.994378513395</v>
+      </c>
+      <c r="D6">
+        <v>195994.28336162199</v>
+      </c>
+      <c r="E6">
+        <v>13.137343095148699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>58323.064570784802</v>
+      </c>
+      <c r="B7">
+        <v>54583.832757687604</v>
+      </c>
+      <c r="C7">
+        <v>83451.4538343819</v>
+      </c>
+      <c r="D7">
+        <v>195998.641944242</v>
+      </c>
+      <c r="E7">
+        <v>12.592544988944701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>58771.869893413299</v>
+      </c>
+      <c r="B8">
+        <v>56221.7927385</v>
+      </c>
+      <c r="C8">
+        <v>87653.419463558501</v>
+      </c>
+      <c r="D8">
+        <v>196002.55469290199</v>
+      </c>
+      <c r="E8">
+        <v>12.1033180330585</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>59044.998413931098</v>
+      </c>
+      <c r="B9">
+        <v>56969.019998109899</v>
+      </c>
+      <c r="C9">
+        <v>91595.097921422494</v>
+      </c>
+      <c r="D9">
+        <v>196004.839076042</v>
+      </c>
+      <c r="E9">
+        <v>11.8159565644017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>59363.532688175699</v>
+      </c>
+      <c r="B10">
+        <v>57880.0448177789</v>
+      </c>
+      <c r="C10">
+        <v>95288.285443637506</v>
+      </c>
+      <c r="D10">
+        <v>196007.80896801199</v>
+      </c>
+      <c r="E10">
+        <v>11.445633673573999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>59052.407578380102</v>
+      </c>
+      <c r="B11">
+        <v>56103.915579560897</v>
+      </c>
+      <c r="C11">
+        <v>97178.729157277994</v>
+      </c>
+      <c r="D11">
+        <v>196003.66064646299</v>
+      </c>
+      <c r="E11">
+        <v>11.9481337588558</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>59311.198362502801</v>
+      </c>
+      <c r="B12">
+        <v>57437.901045510102</v>
+      </c>
+      <c r="C12">
+        <v>100442.56620784001</v>
+      </c>
+      <c r="D12">
+        <v>196008.21596075399</v>
+      </c>
+      <c r="E12">
+        <v>11.383536556373199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>59516.315559038601</v>
+      </c>
+      <c r="B13">
+        <v>58240.332027704499</v>
+      </c>
+      <c r="C13">
+        <v>102984.150171645</v>
+      </c>
+      <c r="D13">
+        <v>196011.34864958699</v>
+      </c>
+      <c r="E13">
+        <v>10.9943996457867</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>59752.107312938599</v>
+      </c>
+      <c r="B14">
+        <v>59092.316776461303</v>
+      </c>
+      <c r="C14">
+        <v>105194.777652594</v>
+      </c>
+      <c r="D14">
+        <v>196014.755075036</v>
+      </c>
+      <c r="E14">
+        <v>10.5714585465968</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>59953.055064619701</v>
+      </c>
+      <c r="B15">
+        <v>59637.500655011798</v>
+      </c>
+      <c r="C15">
+        <v>108736.553572516</v>
+      </c>
+      <c r="D15">
+        <v>196017.25432917001</v>
+      </c>
+      <c r="E15">
+        <v>10.2620357981649</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>60088.145945788601</v>
+      </c>
+      <c r="B16">
+        <v>59847.265382257603</v>
+      </c>
+      <c r="C16">
+        <v>112174.25742574201</v>
+      </c>
+      <c r="D16">
+        <v>196018.608427878</v>
+      </c>
+      <c r="E16">
+        <v>10.0940710666718</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>59808.779814442598</v>
+      </c>
+      <c r="B17">
+        <v>57876.582038628403</v>
+      </c>
+      <c r="C17">
+        <v>113405.21631771101</v>
+      </c>
+      <c r="D17">
+        <v>196012.52704571601</v>
+      </c>
+      <c r="E17">
+        <v>10.8374129087554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>59992.096136334098</v>
+      </c>
+      <c r="B18">
+        <v>58983.755172178498</v>
+      </c>
+      <c r="C18">
+        <v>115859.53726513</v>
+      </c>
+      <c r="D18">
+        <v>196017.088221838</v>
+      </c>
+      <c r="E18">
+        <v>10.2755937896281</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>60185.745003850097</v>
+      </c>
+      <c r="B19">
+        <v>59925.770196199002</v>
+      </c>
+      <c r="C19">
+        <v>117797.302857142</v>
+      </c>
+      <c r="D19">
+        <v>196021.118323578</v>
+      </c>
+      <c r="E19">
+        <v>9.7792430332843896</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>60354.116362750101</v>
+      </c>
+      <c r="B20">
+        <v>60553.844698029003</v>
+      </c>
+      <c r="C20">
+        <v>119690.042619139</v>
+      </c>
+      <c r="D20">
+        <v>196024.039448333</v>
+      </c>
+      <c r="E20">
+        <v>9.4190182184135107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>60504.618254886198</v>
+      </c>
+      <c r="B21">
+        <v>61002.071845092702</v>
+      </c>
+      <c r="C21">
+        <v>121133.374308543</v>
+      </c>
+      <c r="D21">
+        <v>196026.30151917899</v>
+      </c>
+      <c r="E21">
+        <v>9.1400099527017407</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>60647.246062206497</v>
+      </c>
+      <c r="B22">
+        <v>61377.888397682997</v>
+      </c>
+      <c r="C22">
+        <v>122620.029050367</v>
+      </c>
+      <c r="D22">
+        <v>196028.28752524001</v>
+      </c>
+      <c r="E22">
+        <v>8.8952207765615707</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>58371.936477838302</v>
+      </c>
+      <c r="B26">
+        <v>35472.6338299442</v>
+      </c>
+      <c r="C26">
+        <v>76836.395450568598</v>
+      </c>
+      <c r="D26">
+        <v>44968.697598222898</v>
+      </c>
+      <c r="E26">
+        <v>16.2521065819409</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>58632.477552535303</v>
+      </c>
+      <c r="B27">
+        <v>46891.909015302001</v>
+      </c>
+      <c r="C27">
+        <v>76351.363433169405</v>
+      </c>
+      <c r="D27">
+        <v>59664.6144134571</v>
+      </c>
+      <c r="E27">
+        <v>15.1446648453178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>57434.134096442998</v>
+      </c>
+      <c r="B28">
+        <v>46781.641359458001</v>
+      </c>
+      <c r="C28">
+        <v>75564.095525665602</v>
+      </c>
+      <c r="D28">
+        <v>62469.963518078599</v>
+      </c>
+      <c r="E28">
+        <v>15.3397373173395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>57897.471276567499</v>
+      </c>
+      <c r="B29">
+        <v>51679.081666120801</v>
+      </c>
+      <c r="C29">
+        <v>79608.994378513395</v>
+      </c>
+      <c r="D29">
+        <v>73464.123614936107</v>
+      </c>
+      <c r="E29">
+        <v>14.2147463340334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>58323.064570784802</v>
+      </c>
+      <c r="B30">
+        <v>54165.678055017997</v>
+      </c>
+      <c r="C30">
+        <v>83451.4538343819</v>
+      </c>
+      <c r="D30">
+        <v>80120.786501171795</v>
+      </c>
+      <c r="E30">
+        <v>13.542299096154601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>58771.869893413299</v>
+      </c>
+      <c r="B31">
+        <v>55913.8035640944</v>
+      </c>
+      <c r="C31">
+        <v>87653.419463558501</v>
+      </c>
+      <c r="D31">
+        <v>85816.923829635896</v>
+      </c>
+      <c r="E31">
+        <v>13.0016781511156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>59044.998413931098</v>
+      </c>
+      <c r="B32">
+        <v>56690.107258441902</v>
+      </c>
+      <c r="C32">
+        <v>91595.097921422494</v>
+      </c>
+      <c r="D32">
+        <v>90802.5097001127</v>
+      </c>
+      <c r="E32">
+        <v>12.714455258104699</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>59363.532688175699</v>
+      </c>
+      <c r="B33">
+        <v>57611.823533576797</v>
+      </c>
+      <c r="C33">
+        <v>95288.285443637506</v>
+      </c>
+      <c r="D33">
+        <v>95017.304014218302</v>
+      </c>
+      <c r="E33">
+        <v>12.3614266819324</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>59052.407578380102</v>
+      </c>
+      <c r="B34">
+        <v>55884.892749250503</v>
+      </c>
+      <c r="C34">
+        <v>97178.729157277994</v>
+      </c>
+      <c r="D34">
+        <v>97404.860903049397</v>
+      </c>
+      <c r="E34">
+        <v>12.866416065322801</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>59311.198362502801</v>
+      </c>
+      <c r="B35">
+        <v>57180.906105033697</v>
+      </c>
+      <c r="C35">
+        <v>100442.56620784001</v>
+      </c>
+      <c r="D35">
+        <v>100861.251038173</v>
+      </c>
+      <c r="E35">
+        <v>12.346090668886999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>59516.315559038601</v>
+      </c>
+      <c r="B36">
+        <v>57965.174806181902</v>
+      </c>
+      <c r="C36">
+        <v>102984.150171645</v>
+      </c>
+      <c r="D36">
+        <v>103396.49481596801</v>
+      </c>
+      <c r="E36">
+        <v>11.9924747667863</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>59752.107312938599</v>
+      </c>
+      <c r="B37">
+        <v>58804.720089851202</v>
+      </c>
+      <c r="C37">
+        <v>105194.777652594</v>
+      </c>
+      <c r="D37">
+        <v>105460.137963981</v>
+      </c>
+      <c r="E37">
+        <v>11.6023780636563</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>59953.055064619701</v>
+      </c>
+      <c r="B38">
+        <v>59246.679665965799</v>
+      </c>
+      <c r="C38">
+        <v>108736.553572516</v>
+      </c>
+      <c r="D38">
+        <v>109149.99273775201</v>
+      </c>
+      <c r="E38">
+        <v>11.386470849114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>60088.145945788601</v>
+      </c>
+      <c r="B39">
+        <v>59385.210140639399</v>
+      </c>
+      <c r="C39">
+        <v>112174.25742574201</v>
+      </c>
+      <c r="D39">
+        <v>112321.013735801</v>
+      </c>
+      <c r="E39">
+        <v>11.2947603294558</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>59808.779814442598</v>
+      </c>
+      <c r="B40">
+        <v>57501.151901767596</v>
+      </c>
+      <c r="C40">
+        <v>113405.21631771101</v>
+      </c>
+      <c r="D40">
+        <v>114509.091171643</v>
+      </c>
+      <c r="E40">
+        <v>12.0152620533765</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>59992.096136334098</v>
+      </c>
+      <c r="B41">
+        <v>58563.093070461502</v>
+      </c>
+      <c r="C41">
+        <v>115859.53726513</v>
+      </c>
+      <c r="D41">
+        <v>115873.63848181099</v>
+      </c>
+      <c r="E41">
+        <v>11.5019311749676</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>60185.745003850097</v>
+      </c>
+      <c r="B42">
+        <v>59491.434579143701</v>
+      </c>
+      <c r="C42">
+        <v>117797.302857142</v>
+      </c>
+      <c r="D42">
+        <v>116714.037089879</v>
+      </c>
+      <c r="E42">
+        <v>11.0330375794203</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>60354.116362750101</v>
+      </c>
+      <c r="B43">
+        <v>60113.761717786001</v>
+      </c>
+      <c r="C43">
+        <v>119690.042619139</v>
+      </c>
+      <c r="D43">
+        <v>117656.806067122</v>
+      </c>
+      <c r="E43">
+        <v>10.6966136697067</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>60504.618254886198</v>
+      </c>
+      <c r="B44">
+        <v>60570.492187288699</v>
+      </c>
+      <c r="C44">
+        <v>121133.374308543</v>
+      </c>
+      <c r="D44">
+        <v>118317.703158651</v>
+      </c>
+      <c r="E44">
+        <v>10.428129299150299</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>60647.246062206497</v>
+      </c>
+      <c r="B45">
+        <v>60942.730915601802</v>
+      </c>
+      <c r="C45">
+        <v>122620.029050367</v>
+      </c>
+      <c r="D45">
+        <v>119009.154407696</v>
+      </c>
+      <c r="E45">
+        <v>10.1987998575596</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A24:E24"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New experiments with variance or prior for parameters equal to 1
</commit_message>
<xml_diff>
--- a/extensions/icdm2016/doc-Experiments/RecapExperiments.xlsx
+++ b/extensions/icdm2016/doc-Experiments/RecapExperiments.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="0" windowWidth="27320" windowHeight="14000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-25160" yWindow="0" windowWidth="27320" windowHeight="14000" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CajaMar" sheetId="1" r:id="rId1"/>
-    <sheet name="VAR01" sheetId="3" r:id="rId2"/>
+    <sheet name="VAR01-var1e100" sheetId="3" r:id="rId2"/>
+    <sheet name="VAR01-var1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="100">
   <si>
     <t>2016-bs100</t>
   </si>
@@ -1732,6 +1733,1398 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$A$3:$A$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>58371.9364778383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58632.4775525353</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57434.134096443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57897.4712765675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58323.0645707848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58771.8698934133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59044.9984139311</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59363.5326881757</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59052.4075783801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59311.1983625028</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59516.3155590386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59752.1073129386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59953.0550646197</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60088.1459457886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59808.7798144426</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59992.0961363341</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60185.7450038501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60354.1163627501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60504.6182548862</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60647.2460622065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$B$3:$B$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.92627043547087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.32023445123761</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.01706880515186</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.697862261683751</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.4200589946985</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.2759545551717</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.1742574401342</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.1621343748142</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.420621578159</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.6277846616029</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.8968167774719</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.3666342213181</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37.8874626057912</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41.4520798306207</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45.3910060430651</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.3451522829393</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>53.3951264181324</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>57.6983871022685</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.1795811174801</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>66.8794106837971</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2121321448"/>
+        <c:axId val="-2139319480"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2121321448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139319480"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2139319480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2121321448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$C$3:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>76836.3954505686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76351.3634331694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75564.0955256656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79608.99437851339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83451.4538343819</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87653.4194635585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91595.09792142249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95288.2854436375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97178.729157278</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100442.56620784</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102984.150171645</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105194.777652594</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108736.553572516</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>112174.257425742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113405.216317711</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115859.53726513</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>117797.302857142</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>119690.042619139</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121133.374308543</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>122620.029050367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$D$3:$D$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.123904374364694</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.271976766670501</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46547411266136</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.636108132729801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.781116807967592</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.939339130393021</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.09384611210449</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.24033639163669</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.40668730116442</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.56608794818184</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.71594584846476</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.87914445338983</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.05420363935581</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.21306504032643</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.38055333410932</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.52676105952179</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.66169947886676</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.81211399204293</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.95044930231019</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.08868197457224</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2139528520"/>
+        <c:axId val="-2139543000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2139528520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139543000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2139543000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139528520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>meanH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$E$3:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>12.6171813949175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.6231100252224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.6359418074839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.6557085641032</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.6834468739671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.7212913439373</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.7691409336179</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.8285845376442</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.9050132625256</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.9917826943869</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.0916348385833</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.2095178618986</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.3407518376151</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.4845187372158</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.6547079408116</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.8359618224763</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.0310479855886</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.2472343082628</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.4803362892313</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.7319054301708</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="2128395768"/>
+        <c:axId val="-2104583800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2128395768"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2104583800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2104583800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2128395768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$A$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$A$26:$A$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>58371.9364778383</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58632.4775525353</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57434.134096443</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57897.4712765675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58323.0645707848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58771.8698934133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59044.9984139311</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59363.5326881757</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59052.4075783801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59311.1983625028</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>59516.3155590386</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59752.1073129386</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>59953.0550646197</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>60088.1459457886</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59808.7798144426</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>59992.0961363341</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>60185.7450038501</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>60354.1163627501</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>60504.6182548862</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>60647.2460622065</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$B$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$B$26:$B$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.92943809722798</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.3130601514617</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.00373779339924</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.67894305568879</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.3975969848436</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.2499290317774</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.1455040075102</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.1310986101231</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.3860014480484</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>27.5900416433245</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30.8570981880644</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>34.3241992572676</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>37.8434143957806</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41.4071846950887</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45.3415820560583</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>49.2934010688952</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>53.341856825592</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>57.6445436098037</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>62.1237076458415</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>66.82137249108401</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2143783000"/>
+        <c:axId val="2073697000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2143783000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2073697000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2073697000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2143783000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$C$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>realMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$C$26:$C$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>76836.3954505686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76351.3634331694</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75564.0955256656</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79608.99437851339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>83451.4538343819</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87653.4194635585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>91595.09792142249</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>95288.2854436375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97178.729157278</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100442.56620784</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>102984.150171645</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>105194.777652594</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>108736.553572516</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>112174.257425742</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>113405.216317711</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>115859.53726513</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>117797.302857142</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>119690.042619139</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>121133.374308543</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>122620.029050367</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$D$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>learntMean_c1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$D$26:$D$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.11501297200256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.262054903921544</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.455264339211357</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.624779722429832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.769309374221158</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.927104836035391</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.08131004072176</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.22754771566756</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.39377940870687</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.55295578416317</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.70263476619007</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.86569748969329</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.04049451997296</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.19921961599482</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.36640786296067</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.51234952319918</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.64712703370352</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7971430820655</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.93508977618257</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.07292362984796</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2139386936"/>
+        <c:axId val="-2139383656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2139386936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139383656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2139383656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139386936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'VAR01-var1'!$E$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>meanH</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'VAR01-var1'!$E$26:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>12.6172357876381</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.6232129750563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.6360876243457</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.655879971479</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.6836439180836</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.7214996786567</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.7693575195711</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>12.8288074762509</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.9051960302129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.9919204535984</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13.0917464018962</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.209567916076</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.3407698897758</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13.4845263425381</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.6545366836197</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13.835703337263</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14.0307348649372</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14.2469086262423</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14.4799252680995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>14.7314005104666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2139419016"/>
+        <c:axId val="-2139416072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2139419016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139416072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2139416072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2139419016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
@@ -3317,7 +4710,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$A$2</c:f>
+              <c:f>'VAR01-var1e100'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3331,7 +4724,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$A$3:$A$22</c:f>
+              <c:f>'VAR01-var1e100'!$A$3:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3405,7 +4798,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$B$2</c:f>
+              <c:f>'VAR01-var1e100'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3419,7 +4812,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$B$3:$B$22</c:f>
+              <c:f>'VAR01-var1e100'!$B$3:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3577,7 +4970,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$C$2</c:f>
+              <c:f>'VAR01-var1e100'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3591,7 +4984,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$C$3:$C$22</c:f>
+              <c:f>'VAR01-var1e100'!$C$3:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3665,7 +5058,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$D$2</c:f>
+              <c:f>'VAR01-var1e100'!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3679,7 +5072,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$D$3:$D$22</c:f>
+              <c:f>'VAR01-var1e100'!$D$3:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -3841,7 +5234,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$E$2</c:f>
+              <c:f>'VAR01-var1e100'!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3855,7 +5248,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$E$3:$E$22</c:f>
+              <c:f>'VAR01-var1e100'!$E$3:$E$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4013,7 +5406,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$A$25</c:f>
+              <c:f>'VAR01-var1e100'!$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4027,7 +5420,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$A$26:$A$45</c:f>
+              <c:f>'VAR01-var1e100'!$A$26:$A$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4101,7 +5494,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$B$25</c:f>
+              <c:f>'VAR01-var1e100'!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4115,7 +5508,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$B$26:$B$45</c:f>
+              <c:f>'VAR01-var1e100'!$B$26:$B$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4273,7 +5666,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$C$25</c:f>
+              <c:f>'VAR01-var1e100'!$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4287,7 +5680,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$C$26:$C$45</c:f>
+              <c:f>'VAR01-var1e100'!$C$26:$C$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4361,7 +5754,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$D$25</c:f>
+              <c:f>'VAR01-var1e100'!$D$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4375,7 +5768,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$D$26:$D$45</c:f>
+              <c:f>'VAR01-var1e100'!$D$26:$D$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4537,7 +5930,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'VAR01'!$E$25</c:f>
+              <c:f>'VAR01-var1e100'!$E$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4551,7 +5944,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'VAR01'!$E$26:$E$45</c:f>
+              <c:f>'VAR01-var1e100'!$E$26:$E$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4948,6 +6341,203 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="10" name="Chart 9"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -8225,7 +9815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E25" sqref="E25:E45"/>
     </sheetView>
   </sheetViews>
@@ -8961,6 +10551,764 @@
       </c>
       <c r="E45">
         <v>10.1987998575596</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A24:E24"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>58371.936477838302</v>
+      </c>
+      <c r="B3">
+        <v>1.92627043547087</v>
+      </c>
+      <c r="C3">
+        <v>76836.395450568598</v>
+      </c>
+      <c r="D3">
+        <v>0.12390437436469399</v>
+      </c>
+      <c r="E3">
+        <v>12.6171813949175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>58632.477552535303</v>
+      </c>
+      <c r="B4">
+        <v>4.3202344512376101</v>
+      </c>
+      <c r="C4">
+        <v>76351.363433169405</v>
+      </c>
+      <c r="D4">
+        <v>0.27197676667050102</v>
+      </c>
+      <c r="E4">
+        <v>12.623110025222401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>57434.134096442998</v>
+      </c>
+      <c r="B5">
+        <v>7.0170688051518599</v>
+      </c>
+      <c r="C5">
+        <v>75564.095525665602</v>
+      </c>
+      <c r="D5">
+        <v>0.46547411266136002</v>
+      </c>
+      <c r="E5">
+        <v>12.635941807483899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>57897.471276567499</v>
+      </c>
+      <c r="B6">
+        <v>9.6978622616837509</v>
+      </c>
+      <c r="C6">
+        <v>79608.994378513395</v>
+      </c>
+      <c r="D6">
+        <v>0.63610813272980105</v>
+      </c>
+      <c r="E6">
+        <v>12.6557085641032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>58323.064570784802</v>
+      </c>
+      <c r="B7">
+        <v>12.4200589946985</v>
+      </c>
+      <c r="C7">
+        <v>83451.4538343819</v>
+      </c>
+      <c r="D7">
+        <v>0.78111680796759198</v>
+      </c>
+      <c r="E7">
+        <v>12.6834468739671</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>58771.869893413299</v>
+      </c>
+      <c r="B8">
+        <v>15.275954555171699</v>
+      </c>
+      <c r="C8">
+        <v>87653.419463558501</v>
+      </c>
+      <c r="D8">
+        <v>0.93933913039302097</v>
+      </c>
+      <c r="E8">
+        <v>12.721291343937301</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>59044.998413931098</v>
+      </c>
+      <c r="B9">
+        <v>18.174257440134198</v>
+      </c>
+      <c r="C9">
+        <v>91595.097921422494</v>
+      </c>
+      <c r="D9">
+        <v>1.09384611210449</v>
+      </c>
+      <c r="E9">
+        <v>12.7691409336179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>59363.532688175699</v>
+      </c>
+      <c r="B10">
+        <v>21.162134374814201</v>
+      </c>
+      <c r="C10">
+        <v>95288.285443637506</v>
+      </c>
+      <c r="D10">
+        <v>1.2403363916366901</v>
+      </c>
+      <c r="E10">
+        <v>12.8285845376442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>59052.407578380102</v>
+      </c>
+      <c r="B11">
+        <v>24.420621578159</v>
+      </c>
+      <c r="C11">
+        <v>97178.729157277994</v>
+      </c>
+      <c r="D11">
+        <v>1.4066873011644201</v>
+      </c>
+      <c r="E11">
+        <v>12.9050132625256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>59311.198362502801</v>
+      </c>
+      <c r="B12">
+        <v>27.627784661602899</v>
+      </c>
+      <c r="C12">
+        <v>100442.56620784001</v>
+      </c>
+      <c r="D12">
+        <v>1.5660879481818399</v>
+      </c>
+      <c r="E12">
+        <v>12.991782694386901</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>59516.315559038601</v>
+      </c>
+      <c r="B13">
+        <v>30.896816777471901</v>
+      </c>
+      <c r="C13">
+        <v>102984.150171645</v>
+      </c>
+      <c r="D13">
+        <v>1.7159458484647601</v>
+      </c>
+      <c r="E13">
+        <v>13.0916348385833</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>59752.107312938599</v>
+      </c>
+      <c r="B14">
+        <v>34.366634221318101</v>
+      </c>
+      <c r="C14">
+        <v>105194.777652594</v>
+      </c>
+      <c r="D14">
+        <v>1.87914445338983</v>
+      </c>
+      <c r="E14">
+        <v>13.2095178618986</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>59953.055064619701</v>
+      </c>
+      <c r="B15">
+        <v>37.8874626057912</v>
+      </c>
+      <c r="C15">
+        <v>108736.553572516</v>
+      </c>
+      <c r="D15">
+        <v>2.0542036393558099</v>
+      </c>
+      <c r="E15">
+        <v>13.3407518376151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>60088.145945788601</v>
+      </c>
+      <c r="B16">
+        <v>41.452079830620697</v>
+      </c>
+      <c r="C16">
+        <v>112174.25742574201</v>
+      </c>
+      <c r="D16">
+        <v>2.21306504032643</v>
+      </c>
+      <c r="E16">
+        <v>13.484518737215801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>59808.779814442598</v>
+      </c>
+      <c r="B17">
+        <v>45.391006043065097</v>
+      </c>
+      <c r="C17">
+        <v>113405.21631771101</v>
+      </c>
+      <c r="D17">
+        <v>2.3805533341093201</v>
+      </c>
+      <c r="E17">
+        <v>13.654707940811599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>59992.096136334098</v>
+      </c>
+      <c r="B18">
+        <v>49.345152282939303</v>
+      </c>
+      <c r="C18">
+        <v>115859.53726513</v>
+      </c>
+      <c r="D18">
+        <v>2.5267610595217902</v>
+      </c>
+      <c r="E18">
+        <v>13.8359618224763</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>60185.745003850097</v>
+      </c>
+      <c r="B19">
+        <v>53.395126418132399</v>
+      </c>
+      <c r="C19">
+        <v>117797.302857142</v>
+      </c>
+      <c r="D19">
+        <v>2.6616994788667601</v>
+      </c>
+      <c r="E19">
+        <v>14.0310479855886</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>60354.116362750101</v>
+      </c>
+      <c r="B20">
+        <v>57.698387102268498</v>
+      </c>
+      <c r="C20">
+        <v>119690.042619139</v>
+      </c>
+      <c r="D20">
+        <v>2.8121139920429301</v>
+      </c>
+      <c r="E20">
+        <v>14.247234308262801</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>60504.618254886198</v>
+      </c>
+      <c r="B21">
+        <v>62.179581117480097</v>
+      </c>
+      <c r="C21">
+        <v>121133.374308543</v>
+      </c>
+      <c r="D21">
+        <v>2.9504493023101901</v>
+      </c>
+      <c r="E21">
+        <v>14.4803362892313</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>60647.246062206497</v>
+      </c>
+      <c r="B22">
+        <v>66.879410683797104</v>
+      </c>
+      <c r="C22">
+        <v>122620.029050367</v>
+      </c>
+      <c r="D22">
+        <v>3.08868197457224</v>
+      </c>
+      <c r="E22">
+        <v>14.7319054301708</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>58371.936477838302</v>
+      </c>
+      <c r="B26">
+        <v>1.9294380972279801</v>
+      </c>
+      <c r="C26">
+        <v>76836.395450568598</v>
+      </c>
+      <c r="D26">
+        <v>0.11501297200256</v>
+      </c>
+      <c r="E26">
+        <v>12.6172357876381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>58632.477552535303</v>
+      </c>
+      <c r="B27">
+        <v>4.3130601514617002</v>
+      </c>
+      <c r="C27">
+        <v>76351.363433169405</v>
+      </c>
+      <c r="D27">
+        <v>0.26205490392154401</v>
+      </c>
+      <c r="E27">
+        <v>12.623212975056299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28">
+        <v>57434.134096442998</v>
+      </c>
+      <c r="B28">
+        <v>7.0037377933992397</v>
+      </c>
+      <c r="C28">
+        <v>75564.095525665602</v>
+      </c>
+      <c r="D28">
+        <v>0.45526433921135701</v>
+      </c>
+      <c r="E28">
+        <v>12.6360876243457</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29">
+        <v>57897.471276567499</v>
+      </c>
+      <c r="B29">
+        <v>9.6789430556887908</v>
+      </c>
+      <c r="C29">
+        <v>79608.994378513395</v>
+      </c>
+      <c r="D29">
+        <v>0.62477972242983204</v>
+      </c>
+      <c r="E29">
+        <v>12.655879971478999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30">
+        <v>58323.064570784802</v>
+      </c>
+      <c r="B30">
+        <v>12.397596984843601</v>
+      </c>
+      <c r="C30">
+        <v>83451.4538343819</v>
+      </c>
+      <c r="D30">
+        <v>0.76930937422115797</v>
+      </c>
+      <c r="E30">
+        <v>12.6836439180836</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31">
+        <v>58771.869893413299</v>
+      </c>
+      <c r="B31">
+        <v>15.2499290317774</v>
+      </c>
+      <c r="C31">
+        <v>87653.419463558501</v>
+      </c>
+      <c r="D31">
+        <v>0.92710483603539096</v>
+      </c>
+      <c r="E31">
+        <v>12.7214996786567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32">
+        <v>59044.998413931098</v>
+      </c>
+      <c r="B32">
+        <v>18.145504007510201</v>
+      </c>
+      <c r="C32">
+        <v>91595.097921422494</v>
+      </c>
+      <c r="D32">
+        <v>1.08131004072176</v>
+      </c>
+      <c r="E32">
+        <v>12.7693575195711</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33">
+        <v>59363.532688175699</v>
+      </c>
+      <c r="B33">
+        <v>21.1310986101231</v>
+      </c>
+      <c r="C33">
+        <v>95288.285443637506</v>
+      </c>
+      <c r="D33">
+        <v>1.22754771566756</v>
+      </c>
+      <c r="E33">
+        <v>12.828807476250899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34">
+        <v>59052.407578380102</v>
+      </c>
+      <c r="B34">
+        <v>24.3860014480484</v>
+      </c>
+      <c r="C34">
+        <v>97178.729157277994</v>
+      </c>
+      <c r="D34">
+        <v>1.39377940870687</v>
+      </c>
+      <c r="E34">
+        <v>12.905196030212901</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35">
+        <v>59311.198362502801</v>
+      </c>
+      <c r="B35">
+        <v>27.590041643324501</v>
+      </c>
+      <c r="C35">
+        <v>100442.56620784001</v>
+      </c>
+      <c r="D35">
+        <v>1.55295578416317</v>
+      </c>
+      <c r="E35">
+        <v>12.9919204535984</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>59516.315559038601</v>
+      </c>
+      <c r="B36">
+        <v>30.857098188064398</v>
+      </c>
+      <c r="C36">
+        <v>102984.150171645</v>
+      </c>
+      <c r="D36">
+        <v>1.70263476619007</v>
+      </c>
+      <c r="E36">
+        <v>13.0917464018962</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>59752.107312938599</v>
+      </c>
+      <c r="B37">
+        <v>34.324199257267601</v>
+      </c>
+      <c r="C37">
+        <v>105194.777652594</v>
+      </c>
+      <c r="D37">
+        <v>1.8656974896932901</v>
+      </c>
+      <c r="E37">
+        <v>13.209567916076001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>59953.055064619701</v>
+      </c>
+      <c r="B38">
+        <v>37.843414395780599</v>
+      </c>
+      <c r="C38">
+        <v>108736.553572516</v>
+      </c>
+      <c r="D38">
+        <v>2.0404945199729601</v>
+      </c>
+      <c r="E38">
+        <v>13.3407698897758</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>60088.145945788601</v>
+      </c>
+      <c r="B39">
+        <v>41.407184695088702</v>
+      </c>
+      <c r="C39">
+        <v>112174.25742574201</v>
+      </c>
+      <c r="D39">
+        <v>2.1992196159948199</v>
+      </c>
+      <c r="E39">
+        <v>13.4845263425381</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>59808.779814442598</v>
+      </c>
+      <c r="B40">
+        <v>45.3415820560583</v>
+      </c>
+      <c r="C40">
+        <v>113405.21631771101</v>
+      </c>
+      <c r="D40">
+        <v>2.3664078629606702</v>
+      </c>
+      <c r="E40">
+        <v>13.6545366836197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>59992.096136334098</v>
+      </c>
+      <c r="B41">
+        <v>49.2934010688952</v>
+      </c>
+      <c r="C41">
+        <v>115859.53726513</v>
+      </c>
+      <c r="D41">
+        <v>2.5123495231991799</v>
+      </c>
+      <c r="E41">
+        <v>13.835703337263</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>60185.745003850097</v>
+      </c>
+      <c r="B42">
+        <v>53.341856825591996</v>
+      </c>
+      <c r="C42">
+        <v>117797.302857142</v>
+      </c>
+      <c r="D42">
+        <v>2.6471270337035202</v>
+      </c>
+      <c r="E42">
+        <v>14.0307348649372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>60354.116362750101</v>
+      </c>
+      <c r="B43">
+        <v>57.644543609803698</v>
+      </c>
+      <c r="C43">
+        <v>119690.042619139</v>
+      </c>
+      <c r="D43">
+        <v>2.7971430820654999</v>
+      </c>
+      <c r="E43">
+        <v>14.2469086262423</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>60504.618254886198</v>
+      </c>
+      <c r="B44">
+        <v>62.123707645841499</v>
+      </c>
+      <c r="C44">
+        <v>121133.374308543</v>
+      </c>
+      <c r="D44">
+        <v>2.9350897761825698</v>
+      </c>
+      <c r="E44">
+        <v>14.4799252680995</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45">
+        <v>60647.246062206497</v>
+      </c>
+      <c r="B45">
+        <v>66.821372491084006</v>
+      </c>
+      <c r="C45">
+        <v>122620.029050367</v>
+      </c>
+      <c r="D45">
+        <v>3.0729236298479599</v>
+      </c>
+      <c r="E45">
+        <v>14.731400510466599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>